<commit_message>
Add some styles for the msg
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Deporte" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="21">
   <si>
     <t>Deporte</t>
   </si>
@@ -73,6 +73,18 @@
   </si>
   <si>
     <t>Que representan los colores de la bandera Argentina</t>
+  </si>
+  <si>
+    <t>#daa520</t>
+  </si>
+  <si>
+    <t>#db7093</t>
+  </si>
+  <si>
+    <t>#20b2aa</t>
+  </si>
+  <si>
+    <t>#3cb371</t>
   </si>
 </sst>
 </file>
@@ -402,7 +414,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -425,6 +437,9 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -439,6 +454,9 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
@@ -452,6 +470,9 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -465,10 +486,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="A1:D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +497,7 @@
     <col min="3" max="3" width="37.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -489,8 +510,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -503,8 +527,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -516,6 +543,9 @@
       </c>
       <c r="D3" t="s">
         <v>8</v>
+      </c>
+      <c r="E3" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>
@@ -525,10 +555,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -536,7 +566,7 @@
     <col min="3" max="3" width="42.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>13</v>
       </c>
@@ -549,8 +579,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -563,8 +596,11 @@
       <c r="D2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -577,18 +613,22 @@
       <c r="D3" t="s">
         <v>8</v>
       </c>
+      <c r="E3" t="s">
+        <v>17</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -598,7 +638,7 @@
     <col min="4" max="4" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -611,8 +651,11 @@
       <c r="D1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -624,6 +667,9 @@
       </c>
       <c r="D2" t="s">
         <v>8</v>
+      </c>
+      <c r="E2" t="s">
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dificulty selection after spinnig the wheel
</commit_message>
<xml_diff>
--- a/datos.xlsx
+++ b/datos.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
   </bookViews>
   <sheets>
     <sheet name="Deporte" sheetId="1" r:id="rId1"/>
@@ -66,15 +66,6 @@
     <t>Historia</t>
   </si>
   <si>
-    <t>Donde nació Jesús</t>
-  </si>
-  <si>
-    <t>Donde falleció San Martín</t>
-  </si>
-  <si>
-    <t>Que representan los colores de la bandera Argentina</t>
-  </si>
-  <si>
     <t>#daa520</t>
   </si>
   <si>
@@ -85,6 +76,15 @@
   </si>
   <si>
     <t>#3cb371</t>
+  </si>
+  <si>
+    <t>¿Donde nació Jesús?</t>
+  </si>
+  <si>
+    <t>¿Que representan los colores de la bandera Argentina?</t>
+  </si>
+  <si>
+    <t>¿Donde falleció San Martín?</t>
   </si>
 </sst>
 </file>
@@ -413,7 +413,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
@@ -438,7 +438,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -455,7 +455,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -472,7 +472,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -488,7 +488,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -511,7 +511,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -528,7 +528,7 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -545,7 +545,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -558,12 +558,12 @@
   <dimension ref="A1:E3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="42.5703125" customWidth="1"/>
+    <col min="3" max="3" width="71" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
@@ -574,13 +574,13 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>14</v>
+        <v>18</v>
       </c>
       <c r="D1" t="s">
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -591,13 +591,13 @@
         <v>2</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s">
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -608,13 +608,13 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D3" t="s">
         <v>8</v>
       </c>
       <c r="E3" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>
@@ -652,7 +652,7 @@
         <v>7</v>
       </c>
       <c r="E1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -669,7 +669,7 @@
         <v>8</v>
       </c>
       <c r="E2" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>